<commit_message>
update log of builds
</commit_message>
<xml_diff>
--- a/ObjectHandler/dev_tools/builds.xlsx
+++ b/ObjectHandler/dev_tools/builds.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="20">
   <si>
     <t>ObjectHandler_vc?.sln</t>
   </si>
@@ -66,9 +66,6 @@
     <t>VC11 (2012)</t>
   </si>
   <si>
-    <t>VC11 - batch build / rebuild of QuantLibAddin - kick it off in the evening - following morning it's still running.</t>
-  </si>
-  <si>
     <t>TO</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>VC12 (2013)</t>
+  </si>
+  <si>
+    <t>VC11 / VC12 - batch build / rebuild of QuantLibAddin - kick it off in the evening - following morning it's still running.</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
       <c r="R1" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
@@ -799,28 +799,52 @@
         <v>6</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="X6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y6" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -912,10 +936,10 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
         <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -930,21 +954,21 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="R1:Y1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="J1:Q1"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:M2"/>
-    <mergeCell ref="R1:Y1"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="J1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>